<commit_message>
AD_1.3-21 MH AD index chart
updates
</commit_message>
<xml_diff>
--- a/03_AD/csv_xls/honduras_airport_20160331.xlsx
+++ b/03_AD/csv_xls/honduras_airport_20160331.xlsx
@@ -522,9 +522,6 @@
     <t>VILLA GUADALUPE</t>
   </si>
   <si>
-    <t>MHSL</t>
-  </si>
-  <si>
     <t>SAN LORENZO</t>
   </si>
   <si>
@@ -952,6 +949,9 @@
   </si>
   <si>
     <t>aerodrome/heliport name</t>
+  </si>
+  <si>
+    <t>MHSA</t>
   </si>
 </sst>
 </file>
@@ -1795,7 +1795,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H39"/>
+      <selection sqref="A1:H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,36 +1812,36 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>310</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>310</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>310</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>130</v>
@@ -1850,24 +1850,24 @@
         <v>131</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>199</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>274</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>91</v>
@@ -1876,16 +1876,16 @@
         <v>92</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>65</v>
+        <v>19</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1896,10 +1896,10 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>180</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
@@ -1908,24 +1908,24 @@
         <v>11</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>167</v>
+        <v>65</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>168</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>294</v>
-      </c>
       <c r="C5" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>257</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>163</v>
@@ -1934,10 +1934,10 @@
         <v>164</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>214</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1954,10 +1954,10 @@
         <v>158</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>152</v>
@@ -1986,10 +1986,10 @@
         <v>121</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>246</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2006,10 +2006,10 @@
         <v>133</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>85</v>
@@ -2032,16 +2032,16 @@
         <v>129</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>237</v>
-      </c>
       <c r="G9" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>234</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2072,10 +2072,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>
@@ -2084,16 +2084,16 @@
         <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>170</v>
-      </c>
       <c r="G11" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2124,10 +2124,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>116</v>
@@ -2136,10 +2136,10 @@
         <v>117</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>83</v>
@@ -2156,10 +2156,10 @@
         <v>125</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>291</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>292</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>93</v>
@@ -2194,15 +2194,15 @@
         <v>101</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>156</v>
@@ -2220,18 +2220,18 @@
         <v>119</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>136</v>
@@ -2240,10 +2240,10 @@
         <v>137</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>4</v>
@@ -2254,10 +2254,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>279</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>280</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>95</v>
@@ -2266,24 +2266,24 @@
         <v>96</v>
       </c>
       <c r="E18" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>264</v>
-      </c>
       <c r="G18" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>295</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>229</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>47</v>
@@ -2298,18 +2298,18 @@
         <v>15</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>233</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>37</v>
@@ -2318,24 +2318,24 @@
         <v>38</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>227</v>
-      </c>
       <c r="G20" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>29</v>
@@ -2344,10 +2344,10 @@
         <v>30</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>49</v>
@@ -2370,10 +2370,10 @@
         <v>32</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>297</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>298</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>110</v>
@@ -2390,16 +2390,16 @@
         <v>155</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="E23" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>281</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>282</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>97</v>
@@ -2410,16 +2410,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>197</v>
-      </c>
       <c r="C24" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>2</v>
@@ -2436,10 +2436,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>142</v>
@@ -2448,10 +2448,10 @@
         <v>143</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>114</v>
@@ -2468,16 +2468,16 @@
         <v>90</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>270</v>
-      </c>
       <c r="E26" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>278</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>165</v>
@@ -2506,10 +2506,10 @@
         <v>9</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>275</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2532,18 +2532,18 @@
         <v>151</v>
       </c>
       <c r="G28" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>108</v>
@@ -2552,27 +2552,27 @@
         <v>109</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>221</v>
-      </c>
       <c r="G29" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>303</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>231</v>
-      </c>
       <c r="C30" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>28</v>
@@ -2584,24 +2584,24 @@
         <v>26</v>
       </c>
       <c r="G30" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>262</v>
-      </c>
       <c r="C31" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>283</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>284</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>59</v>
@@ -2610,18 +2610,18 @@
         <v>60</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>266</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>6</v>
@@ -2630,24 +2630,24 @@
         <v>7</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>300</v>
-      </c>
       <c r="G32" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="H32" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>35</v>
@@ -2662,10 +2662,10 @@
         <v>54</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2676,30 +2676,30 @@
         <v>80</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>288</v>
-      </c>
       <c r="E34" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>202</v>
-      </c>
       <c r="G34" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>23</v>
@@ -2714,10 +2714,10 @@
         <v>72</v>
       </c>
       <c r="G35" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="H35" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2734,16 +2734,16 @@
         <v>113</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>272</v>
-      </c>
       <c r="G36" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="H36" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2754,16 +2754,16 @@
         <v>76</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>286</v>
-      </c>
       <c r="E37" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2788,10 +2788,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>206</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>55</v>
@@ -2800,18 +2800,18 @@
         <v>56</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>289</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>290</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>161</v>
@@ -2820,10 +2820,10 @@
         <v>162</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>43</v>
+        <v>310</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>44</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2840,15 +2840,15 @@
         <v>160</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B158">
-    <sortCondition ref="A2"/>
+  <sortState ref="J9:J16">
+    <sortCondition ref="J9"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>